<commit_message>
update fos 0.2 14
</commit_message>
<xml_diff>
--- a/Benchmark_System/MAX SENSITIVITY 1.4/Fourth Order System0.2_ms14/Fourth Order System0.2_ms2_latex.xlsx
+++ b/Benchmark_System/MAX SENSITIVITY 1.4/Fourth Order System0.2_ms14/Fourth Order System0.2_ms2_latex.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>parametri</t>
   </si>
@@ -78,28 +78,25 @@
     <t>PID</t>
   </si>
   <si>
-    <t>$C(s) =\frac{3.11\,s^2+16.39\,s+13.47}{0.002226\,s^2+1.215\,s}$</t>
+    <t>$C(s) =\frac{3.174\,s^2+16.08\,s+13.18}{0.0023\,s^2+1.219\,s}$</t>
   </si>
   <si>
     <t>IPD</t>
   </si>
   <si>
-    <t>$C_1(s) =\frac{568.2}{s}$  $C_2(s) =\frac{8.028\,s+101.6}{0.002031\,s+1.0}$</t>
+    <t>$C_1(s) =\frac{3.631}{s}$  $C_2(s) =\frac{2.826\,s+6.76}{0.02427\,s+1.0}$</t>
   </si>
   <si>
     <t>DPI</t>
   </si>
   <si>
-    <t>$C_1(s) =1.05$  $C_2(s) =\frac{0.3281}{s}$  $C_3(s) =\frac{0.42\,s}{0.02667\,s+1.0}$</t>
+    <t>$C_1(s) =4.4585$  $C_2(s) =\frac{0.6278}{s}$  $C_3(s) =\frac{1.823\,s}{0.01132\,s+1.0}$</t>
   </si>
   <si>
     <t>PIDA</t>
   </si>
   <si>
-    <t>$C(s) =\frac{0.002898\,s^4+1.017\,s^3+11.53\,s^2+39.13\,s+29.13}{4.293e-10\,s^4+2.72e-6\,s^3+0.004742\,s^2+1.34\,s}$</t>
-  </si>
-  <si>
-    <t>$C_1(s) =29.0998$  $C_2(s) =\frac{4.811}{s}$  $C_3(s) =\frac{4.836\,s}{0.0065\,s+1.0}$</t>
+    <t>$C(s) =\frac{0.002797\,s^4+1.3\,s^3+20.24\,s^2+83.19\,s+64.24}{8.676e-11\,s^4+1.025e-6\,s^3+0.00325\,s^2+1.293\,s}$</t>
   </si>
 </sst>
 </file>
@@ -120,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -130,18 +127,14 @@
     </border>
     <border/>
     <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,124 +148,124 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="true"/>
-    <col min="2" max="2" width="56" customWidth="true"/>
-    <col min="3" max="3" width="65" customWidth="true"/>
-    <col min="4" max="4" width="73.7109375" customWidth="true"/>
-    <col min="5" max="5" width="104.140625" customWidth="true"/>
+    <col min="2" max="2" width="55" customWidth="true"/>
+    <col min="3" max="3" width="63" customWidth="true"/>
+    <col min="4" max="4" width="74.7109375" customWidth="true"/>
+    <col min="5" max="5" width="103.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.10069246293948622</v>
+        <v>0.10109578804696412</v>
       </c>
       <c r="C3">
-        <v>0.19925649227589393</v>
+        <v>2.1374021739348059</v>
       </c>
       <c r="D3">
-        <v>0.20792512726294152</v>
+        <v>1.5929736852202085</v>
       </c>
       <c r="E3">
-        <v>0.046857663798940442</v>
+        <v>0.020838485521172914</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>13.469981589604442</v>
+        <v>13.175118108275534</v>
       </c>
       <c r="C4">
-        <v>101.560398591387</v>
+        <v>6.7601334600593184</v>
       </c>
       <c r="D4">
-        <v>29.0997995109139</v>
+        <v>4.4585431936982811</v>
       </c>
       <c r="E4">
-        <v>29.131527825605154</v>
+        <v>64.238932755179121</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1.2152787251282979</v>
+        <v>1.218692506687403</v>
       </c>
       <c r="C5">
-        <v>0.17873183297102099</v>
+        <v>1.861924929648904</v>
       </c>
       <c r="D5">
-        <v>6.04912452680251</v>
+        <v>7.1021397489810179</v>
       </c>
       <c r="E5">
-        <v>1.3396083441121001</v>
+        <v>1.2925635821932677</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.188138612520061</v>
+        <v>0.195780770592273</v>
       </c>
       <c r="C6">
-        <v>0.077015531050712002</v>
+        <v>0.39370388968740699</v>
       </c>
       <c r="D6">
-        <v>0.16619495714040899</v>
+        <v>0.40893142255738102</v>
       </c>
       <c r="E6">
-        <v>0.29189719085638499</v>
+        <v>0.24129851120039555</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E7">
-        <v>0.025851369157554999</v>
+        <v>0.015574343636600292</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -289,7 +282,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -306,100 +299,100 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>102.7294742576705</v>
+        <v>103.7209327665792</v>
       </c>
       <c r="C10">
-        <v>37.914855379493197</v>
+        <v>16.222375069598719</v>
       </c>
       <c r="D10">
-        <v>25.5673162636526</v>
+        <v>36.129690930396485</v>
       </c>
       <c r="E10">
-        <v>101.6576260314649</v>
+        <v>111.58996146053157</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11">
-        <v>77.37843986667734</v>
+        <v>88.397527344577796</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1.3999966453466786</v>
+        <v>1.3999995754524437</v>
       </c>
       <c r="C12">
-        <v>1.3999556206374486</v>
+        <v>1.1590725796863817</v>
       </c>
       <c r="D12">
-        <v>1.3999550695564393</v>
+        <v>1.1165562229787664</v>
       </c>
       <c r="E12">
-        <v>1.3211876421343995</v>
+        <v>1.3999899061207535</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.11326633120053087</v>
+        <v>0.11301156132123021</v>
       </c>
       <c r="C13">
-        <v>0.23614724462734213</v>
+        <v>3.60140564251454</v>
       </c>
       <c r="D13">
-        <v>0.35786448936387183</v>
+        <v>2.5637228096197058</v>
       </c>
       <c r="E13">
-        <v>0.022842427745154978</v>
+        <v>0.015122524846155751</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.30239910895573668</v>
+        <v>0.48068989011372149</v>
       </c>
       <c r="C14">
-        <v>0.70652099985492423</v>
+        <v>6.4460571862463647</v>
       </c>
       <c r="D14">
-        <v>0.70919466226707584</v>
+        <v>15.310819017254429</v>
       </c>
       <c r="E14">
-        <v>0.45423465977862471</v>
+        <v>0.19386120511433746</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>5.0212608272448556</v>
+        <v>4.2640505337536716</v>
       </c>
       <c r="C15">
-        <v>4.7951427508317934</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>3.6823269017976612</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -416,71 +409,71 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1.0502126082724486</v>
+        <v>1.0426405053375365</v>
       </c>
       <c r="C17">
-        <v>1.0479514275083179</v>
+        <v>0.99912880337904664</v>
       </c>
       <c r="D17">
-        <v>0.99967855374276571</v>
+        <v>0.99942353561422681</v>
       </c>
       <c r="E17">
-        <v>0.99844557025614467</v>
+        <v>1.0368232690179766</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.2361234792098888</v>
+        <v>0.23033952318255399</v>
       </c>
       <c r="C18">
-        <v>0.46182032933894157</v>
+        <v>10.802845232701818</v>
       </c>
       <c r="D18">
-        <v>1.4360758961179856</v>
+        <v>44.025881970460809</v>
       </c>
       <c r="E18">
-        <v>0.88979564005968648</v>
+        <v>0.029604821498780413</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>9.5990562093617164</v>
+        <v>9.4641072432786117</v>
       </c>
       <c r="C19">
-        <v>3.5935827159001943</v>
+        <v>38.295282709793206</v>
       </c>
       <c r="D19">
-        <v>3.8302963713192528</v>
+        <v>14.402026366559678</v>
       </c>
       <c r="E19">
-        <v>20.256661998342011</v>
+        <v>28.041576530166026</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>62.371925411014317</v>
+        <v>62.928504501873149</v>
       </c>
       <c r="C20">
-        <v>63.928928491885635</v>
+        <v>76.944318229849955</v>
       </c>
       <c r="D20">
-        <v>79.254117041990469</v>
+        <v>90.831736111463073</v>
       </c>
       <c r="E20">
-        <v>70.710505430734798</v>
+        <v>60.213184619523339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>